<commit_message>
update code và giao diện
</commit_message>
<xml_diff>
--- a/omr-backend/grade/grade.xlsx
+++ b/omr-backend/grade/grade.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>MA SINH VIEN</t>
   </si>
@@ -25,10 +25,16 @@
     <t>DIEM</t>
   </si>
   <si>
-    <t>752100</t>
-  </si>
-  <si>
-    <t>106</t>
+    <t>SO CAU DUNG</t>
+  </si>
+  <si>
+    <t>TONG CAU</t>
+  </si>
+  <si>
+    <t>301111</t>
+  </si>
+  <si>
+    <t>110</t>
   </si>
 </sst>
 </file>
@@ -386,13 +392,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -402,16 +408,28 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2">
-        <v>4.17</v>
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>50</v>
+      </c>
+      <c r="E2">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>